<commit_message>
Restructuring of tir.fits() and tir.robustness()
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\tubCloud\MA\TG_IR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Documents\GitHub\TGA-FTIR-hyphenation-tool-kit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A70D090-3A7B-47F5-B85A-BD1487DA1945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA940BA-5707-4B22-B5DC-107A7FEF8071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
   <sheets>
     <sheet name="center_0" sheetId="1" r:id="rId1"/>
@@ -23,33 +23,19 @@
     <sheet name="hwhm_max" sheetId="6" r:id="rId8"/>
     <sheet name="height_max" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>figueiredo1999</t>
-  </si>
-  <si>
-    <t>co2</t>
-  </si>
-  <si>
-    <t>co</t>
   </si>
   <si>
     <t>anhydrides</t>
@@ -112,9 +98,6 @@
     <t>carbonyls 2</t>
   </si>
   <si>
-    <t>h2o</t>
-  </si>
-  <si>
     <t>gas</t>
   </si>
   <si>
@@ -149,6 +132,18 @@
   </si>
   <si>
     <t>almarri2009b</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>H2O</t>
   </si>
 </sst>
 </file>
@@ -550,157 +545,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E64D511-D4ED-4E7F-BCBD-B5A2B90CC7A9}">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="6"/>
-    <col min="2" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="6"/>
+    <col min="2" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="T2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>250</v>
@@ -730,9 +725,9 @@
         <v>840</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1">
         <v>390</v>
@@ -768,7 +763,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -788,9 +783,9 @@
         <v>807</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>267</v>
@@ -814,9 +809,9 @@
         <v>847</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
         <v>257</v>
@@ -840,9 +835,9 @@
         <v>797</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <v>245</v>
@@ -881,9 +876,9 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>263.66666666666663</v>
@@ -910,9 +905,9 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>280</v>
@@ -948,9 +943,9 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
         <v>291</v>
@@ -971,9 +966,9 @@
         <v>775</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1">
         <v>427</v>
@@ -994,9 +989,9 @@
         <v>677</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1">
         <v>275</v>
@@ -1032,9 +1027,9 @@
         <v>930</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1">
         <v>95</v>
@@ -1079,9 +1074,9 @@
         <v>960</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>95</v>
@@ -1132,9 +1127,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>95</v>
@@ -1177,6 +1172,20 @@
       </c>
       <c r="T16" s="1">
         <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1">
+        <v>245</v>
+      </c>
+      <c r="D17" s="1">
+        <v>380</v>
+      </c>
+      <c r="E17" s="1">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1195,9 +1204,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -1391,94 +1400,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -1581,235 +1590,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -1828,9 +1837,9 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -2024,94 +2033,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -2210,235 +2219,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -2457,9 +2466,9 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -2653,94 +2662,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -2843,235 +2852,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -3090,9 +3099,9 @@
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -3286,94 +3295,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -3476,223 +3485,223 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
@@ -3882,7 +3891,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
@@ -4072,7 +4081,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -4275,9 +4284,9 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -4471,94 +4480,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -4661,235 +4670,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -4908,9 +4917,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -5104,94 +5113,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -5294,235 +5303,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -5541,9 +5550,9 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -5737,94 +5746,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -5927,235 +5936,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>
@@ -6174,9 +6183,9 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
         <v>group</v>
@@ -6370,94 +6379,94 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
         <v>gas</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>co2</v>
+        <v>CO2</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="N2" t="str">
         <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="P2" t="str">
         <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="R2" t="str">
         <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="S2" t="str">
         <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>co</v>
+        <v>CO</v>
       </c>
       <c r="T2" t="str">
         <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="U2" t="str">
         <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="V2" t="str">
         <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>h2o</v>
+        <v>H2O</v>
       </c>
       <c r="W2" t="str">
         <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
@@ -6560,235 +6569,235 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
         <v>almarri2009</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
         <v>ducuosso2015</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
         <v>figueiredo1999</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
         <v>figueiredo2007</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
         <v>gorghulo2008</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
         <v>li2011</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
         <v>morales2014</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
         <v>na2011</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
         <v>samant2004</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
         <v>szymanski2002</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
         <v>zhou2007</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
         <v>almarri2009b</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
         <v/>

</xml_diff>

<commit_message>
Added functionality to fits() and major rework and restructuring.
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Documents\GitHub\TGA-FTIR-hyphenation-tool-kit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA940BA-5707-4B22-B5DC-107A7FEF8071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CCDB66-6FB6-4972-B182-F716BFA6F762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
   <sheets>
     <sheet name="center_0" sheetId="1" r:id="rId1"/>
-    <sheet name="hwhm_0" sheetId="3" r:id="rId2"/>
-    <sheet name="height_0" sheetId="2" r:id="rId3"/>
-    <sheet name="center_min" sheetId="5" r:id="rId4"/>
-    <sheet name="hwhm_min" sheetId="4" r:id="rId5"/>
-    <sheet name="height_min" sheetId="7" r:id="rId6"/>
-    <sheet name="center_max" sheetId="9" r:id="rId7"/>
-    <sheet name="hwhm_max" sheetId="6" r:id="rId8"/>
-    <sheet name="height_max" sheetId="8" r:id="rId9"/>
+    <sheet name="link" sheetId="10" r:id="rId2"/>
+    <sheet name="hwhm_0" sheetId="3" r:id="rId3"/>
+    <sheet name="height_0" sheetId="2" r:id="rId4"/>
+    <sheet name="center_min" sheetId="5" r:id="rId5"/>
+    <sheet name="hwhm_min" sheetId="4" r:id="rId6"/>
+    <sheet name="height_min" sheetId="7" r:id="rId7"/>
+    <sheet name="center_max" sheetId="9" r:id="rId8"/>
+    <sheet name="hwhm_max" sheetId="6" r:id="rId9"/>
+    <sheet name="height_max" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>figueiredo1999</t>
   </si>
@@ -134,9 +135,6 @@
     <t>almarri2009b</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
@@ -222,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -231,6 +229,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -547,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E64D511-D4ED-4E7F-BCBD-B5A2B90CC7A9}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,67 +629,67 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1174,19 +1173,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="1">
-        <v>245</v>
-      </c>
-      <c r="D17" s="1">
-        <v>380</v>
-      </c>
-      <c r="E17" s="1">
-        <v>500</v>
-      </c>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F17" s="8"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V13">
@@ -1196,7 +1186,1273 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C02276-5893-45C5-8032-5F138C27CB79}">
+  <dimension ref="A1:AV41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
+        <v>group</v>
+      </c>
+      <c r="B1" t="str">
+        <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
+        <v>adsorbed</v>
+      </c>
+      <c r="C1" t="str">
+        <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
+        <v>carboxylic 1</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
+        <v>carboxylic 2</v>
+      </c>
+      <c r="E1" t="str">
+        <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
+        <v>anhydrides</v>
+      </c>
+      <c r="F1" t="str">
+        <f>IF(ISBLANK(center_0!F1),"",center_0!F1)</f>
+        <v>peroxides</v>
+      </c>
+      <c r="G1" t="str">
+        <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
+        <v>unassigned</v>
+      </c>
+      <c r="H1" t="str">
+        <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
+        <v>lactones 1</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
+        <v>lactones 2</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
+        <v>carbonyl 1</v>
+      </c>
+      <c r="K1" t="str">
+        <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
+        <v>carboxylic 1</v>
+      </c>
+      <c r="L1" t="str">
+        <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
+        <v>carboxylic 2</v>
+      </c>
+      <c r="M1" t="str">
+        <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
+        <v>anhydrides</v>
+      </c>
+      <c r="N1" t="str">
+        <f>IF(ISBLANK(center_0!N1),"",center_0!N1)</f>
+        <v>hydroxyl</v>
+      </c>
+      <c r="O1" t="str">
+        <f>IF(ISBLANK(center_0!O1),"",center_0!O1)</f>
+        <v>phenols</v>
+      </c>
+      <c r="P1" t="str">
+        <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
+        <v>carbonyls 1</v>
+      </c>
+      <c r="Q1" t="str">
+        <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
+        <v>carbonyls 2</v>
+      </c>
+      <c r="R1" t="str">
+        <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
+        <v>ether</v>
+      </c>
+      <c r="S1" t="str">
+        <f>IF(ISBLANK(center_0!S1),"",center_0!S1)</f>
+        <v>pyrones</v>
+      </c>
+      <c r="T1" t="str">
+        <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
+        <v>adsorbed</v>
+      </c>
+      <c r="U1" t="str">
+        <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
+        <v>unassigned 1</v>
+      </c>
+      <c r="V1" t="str">
+        <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
+        <v>unassigned 2</v>
+      </c>
+      <c r="W1" t="str">
+        <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
+        <v/>
+      </c>
+      <c r="X1" t="str">
+        <f>IF(ISBLANK(center_0!X1),"",center_0!X1)</f>
+        <v/>
+      </c>
+      <c r="Y1" t="str">
+        <f>IF(ISBLANK(center_0!Y1),"",center_0!Y1)</f>
+        <v/>
+      </c>
+      <c r="Z1" t="str">
+        <f>IF(ISBLANK(center_0!Z1),"",center_0!Z1)</f>
+        <v/>
+      </c>
+      <c r="AA1" t="str">
+        <f>IF(ISBLANK(center_0!AA1),"",center_0!AA1)</f>
+        <v/>
+      </c>
+      <c r="AB1" t="str">
+        <f>IF(ISBLANK(center_0!AB1),"",center_0!AB1)</f>
+        <v/>
+      </c>
+      <c r="AC1" t="str">
+        <f>IF(ISBLANK(center_0!AC1),"",center_0!AC1)</f>
+        <v/>
+      </c>
+      <c r="AD1" t="str">
+        <f>IF(ISBLANK(center_0!AD1),"",center_0!AD1)</f>
+        <v/>
+      </c>
+      <c r="AE1" t="str">
+        <f>IF(ISBLANK(center_0!AE1),"",center_0!AE1)</f>
+        <v/>
+      </c>
+      <c r="AF1" t="str">
+        <f>IF(ISBLANK(center_0!AF1),"",center_0!AF1)</f>
+        <v/>
+      </c>
+      <c r="AG1" t="str">
+        <f>IF(ISBLANK(center_0!AG1),"",center_0!AG1)</f>
+        <v/>
+      </c>
+      <c r="AH1" t="str">
+        <f>IF(ISBLANK(center_0!AH1),"",center_0!AH1)</f>
+        <v/>
+      </c>
+      <c r="AI1" t="str">
+        <f>IF(ISBLANK(center_0!AI1),"",center_0!AI1)</f>
+        <v/>
+      </c>
+      <c r="AJ1" t="str">
+        <f>IF(ISBLANK(center_0!AJ1),"",center_0!AJ1)</f>
+        <v/>
+      </c>
+      <c r="AK1" t="str">
+        <f>IF(ISBLANK(center_0!AK1),"",center_0!AK1)</f>
+        <v/>
+      </c>
+      <c r="AL1" t="str">
+        <f>IF(ISBLANK(center_0!AL1),"",center_0!AL1)</f>
+        <v/>
+      </c>
+      <c r="AM1" t="str">
+        <f>IF(ISBLANK(center_0!AM1),"",center_0!AM1)</f>
+        <v/>
+      </c>
+      <c r="AN1" t="str">
+        <f>IF(ISBLANK(center_0!AN1),"",center_0!AN1)</f>
+        <v/>
+      </c>
+      <c r="AO1" t="str">
+        <f>IF(ISBLANK(center_0!AO1),"",center_0!AO1)</f>
+        <v/>
+      </c>
+      <c r="AP1" t="str">
+        <f>IF(ISBLANK(center_0!AP1),"",center_0!AP1)</f>
+        <v/>
+      </c>
+      <c r="AQ1" t="str">
+        <f>IF(ISBLANK(center_0!AQ1),"",center_0!AQ1)</f>
+        <v/>
+      </c>
+      <c r="AR1" t="str">
+        <f>IF(ISBLANK(center_0!AR1),"",center_0!AR1)</f>
+        <v/>
+      </c>
+      <c r="AS1" t="str">
+        <f>IF(ISBLANK(center_0!AS1),"",center_0!AS1)</f>
+        <v/>
+      </c>
+      <c r="AT1" t="str">
+        <f>IF(ISBLANK(center_0!AT1),"",center_0!AT1)</f>
+        <v/>
+      </c>
+      <c r="AU1" t="str">
+        <f>IF(ISBLANK(center_0!AU1),"",center_0!AU1)</f>
+        <v/>
+      </c>
+      <c r="AV1" t="str">
+        <f>IF(ISBLANK(center_0!AV1),"",center_0!AV1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
+        <v>gas</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
+        <v>CO</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
+        <v>CO</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
+        <v>CO</v>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
+        <v>CO</v>
+      </c>
+      <c r="O2" t="str">
+        <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
+        <v>CO</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
+        <v>CO</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
+        <v>CO</v>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
+        <v>CO</v>
+      </c>
+      <c r="S2" t="str">
+        <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
+        <v>CO</v>
+      </c>
+      <c r="T2" t="str">
+        <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
+        <v>H2O</v>
+      </c>
+      <c r="U2" t="str">
+        <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
+        <v>H2O</v>
+      </c>
+      <c r="V2" t="str">
+        <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
+        <v>H2O</v>
+      </c>
+      <c r="W2" t="str">
+        <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
+        <v/>
+      </c>
+      <c r="X2" t="str">
+        <f>IF(ISBLANK(center_0!X2),"",center_0!X2)</f>
+        <v/>
+      </c>
+      <c r="Y2" t="str">
+        <f>IF(ISBLANK(center_0!Y2),"",center_0!Y2)</f>
+        <v/>
+      </c>
+      <c r="Z2" t="str">
+        <f>IF(ISBLANK(center_0!Z2),"",center_0!Z2)</f>
+        <v/>
+      </c>
+      <c r="AA2" t="str">
+        <f>IF(ISBLANK(center_0!AA2),"",center_0!AA2)</f>
+        <v/>
+      </c>
+      <c r="AB2" t="str">
+        <f>IF(ISBLANK(center_0!AB2),"",center_0!AB2)</f>
+        <v/>
+      </c>
+      <c r="AC2" t="str">
+        <f>IF(ISBLANK(center_0!AC2),"",center_0!AC2)</f>
+        <v/>
+      </c>
+      <c r="AD2" t="str">
+        <f>IF(ISBLANK(center_0!AD2),"",center_0!AD2)</f>
+        <v/>
+      </c>
+      <c r="AE2" t="str">
+        <f>IF(ISBLANK(center_0!AE2),"",center_0!AE2)</f>
+        <v/>
+      </c>
+      <c r="AF2" t="str">
+        <f>IF(ISBLANK(center_0!AF2),"",center_0!AF2)</f>
+        <v/>
+      </c>
+      <c r="AG2" t="str">
+        <f>IF(ISBLANK(center_0!AG2),"",center_0!AG2)</f>
+        <v/>
+      </c>
+      <c r="AH2" t="str">
+        <f>IF(ISBLANK(center_0!AH2),"",center_0!AH2)</f>
+        <v/>
+      </c>
+      <c r="AI2" t="str">
+        <f>IF(ISBLANK(center_0!AI2),"",center_0!AI2)</f>
+        <v/>
+      </c>
+      <c r="AJ2" t="str">
+        <f>IF(ISBLANK(center_0!AJ2),"",center_0!AJ2)</f>
+        <v/>
+      </c>
+      <c r="AK2" t="str">
+        <f>IF(ISBLANK(center_0!AK2),"",center_0!AK2)</f>
+        <v/>
+      </c>
+      <c r="AL2" t="str">
+        <f>IF(ISBLANK(center_0!AL2),"",center_0!AL2)</f>
+        <v/>
+      </c>
+      <c r="AM2" t="str">
+        <f>IF(ISBLANK(center_0!AM2),"",center_0!AM2)</f>
+        <v/>
+      </c>
+      <c r="AN2" t="str">
+        <f>IF(ISBLANK(center_0!AN2),"",center_0!AN2)</f>
+        <v/>
+      </c>
+      <c r="AO2" t="str">
+        <f>IF(ISBLANK(center_0!AO2),"",center_0!AO2)</f>
+        <v/>
+      </c>
+      <c r="AP2" t="str">
+        <f>IF(ISBLANK(center_0!AP2),"",center_0!AP2)</f>
+        <v/>
+      </c>
+      <c r="AQ2" t="str">
+        <f>IF(ISBLANK(center_0!AQ2),"",center_0!AQ2)</f>
+        <v/>
+      </c>
+      <c r="AR2" t="str">
+        <f>IF(ISBLANK(center_0!AR2),"",center_0!AR2)</f>
+        <v/>
+      </c>
+      <c r="AS2" t="str">
+        <f>IF(ISBLANK(center_0!AS2),"",center_0!AS2)</f>
+        <v/>
+      </c>
+      <c r="AT2" t="str">
+        <f>IF(ISBLANK(center_0!AT2),"",center_0!AT2)</f>
+        <v/>
+      </c>
+      <c r="AU2" t="str">
+        <f>IF(ISBLANK(center_0!AU2),"",center_0!AU2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
+        <v>almarri2009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
+        <v>ducuosso2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
+        <v>figueiredo1999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
+        <v>figueiredo2007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
+        <v>gorghulo2008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
+        <v>li2011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
+        <v>morales2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
+        <v>na2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
+        <v>samant2004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
+        <v>szymanski2002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
+        <v>zhou2007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
+        <v>almarri2009b</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
+        <v>saal2020a</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
+        <v>saal2020b</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55AB40E-2FFC-42C2-AD78-D9FFEE5C8809}">
+  <dimension ref="A1:AV41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
+        <v>group</v>
+      </c>
+      <c r="B1" t="str">
+        <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
+        <v>adsorbed</v>
+      </c>
+      <c r="C1" t="str">
+        <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
+        <v>carboxylic 1</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
+        <v>carboxylic 2</v>
+      </c>
+      <c r="E1" t="str">
+        <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
+        <v>anhydrides</v>
+      </c>
+      <c r="F1" t="str">
+        <f>IF(ISBLANK(center_0!F1),"",center_0!F1)</f>
+        <v>peroxides</v>
+      </c>
+      <c r="G1" t="str">
+        <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
+        <v>unassigned</v>
+      </c>
+      <c r="H1" t="str">
+        <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
+        <v>lactones 1</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
+        <v>lactones 2</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
+        <v>carbonyl 1</v>
+      </c>
+      <c r="K1" t="str">
+        <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
+        <v>carboxylic 1</v>
+      </c>
+      <c r="L1" t="str">
+        <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
+        <v>carboxylic 2</v>
+      </c>
+      <c r="M1" t="str">
+        <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
+        <v>anhydrides</v>
+      </c>
+      <c r="N1" t="str">
+        <f>IF(ISBLANK(center_0!N1),"",center_0!N1)</f>
+        <v>hydroxyl</v>
+      </c>
+      <c r="O1" t="str">
+        <f>IF(ISBLANK(center_0!O1),"",center_0!O1)</f>
+        <v>phenols</v>
+      </c>
+      <c r="P1" t="str">
+        <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
+        <v>carbonyls 1</v>
+      </c>
+      <c r="Q1" t="str">
+        <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
+        <v>carbonyls 2</v>
+      </c>
+      <c r="R1" t="str">
+        <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
+        <v>ether</v>
+      </c>
+      <c r="S1" t="str">
+        <f>IF(ISBLANK(center_0!S1),"",center_0!S1)</f>
+        <v>pyrones</v>
+      </c>
+      <c r="T1" t="str">
+        <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
+        <v>adsorbed</v>
+      </c>
+      <c r="U1" t="str">
+        <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
+        <v>unassigned 1</v>
+      </c>
+      <c r="V1" t="str">
+        <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
+        <v>unassigned 2</v>
+      </c>
+      <c r="W1" t="str">
+        <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
+        <v/>
+      </c>
+      <c r="X1" t="str">
+        <f>IF(ISBLANK(center_0!X1),"",center_0!X1)</f>
+        <v/>
+      </c>
+      <c r="Y1" t="str">
+        <f>IF(ISBLANK(center_0!Y1),"",center_0!Y1)</f>
+        <v/>
+      </c>
+      <c r="Z1" t="str">
+        <f>IF(ISBLANK(center_0!Z1),"",center_0!Z1)</f>
+        <v/>
+      </c>
+      <c r="AA1" t="str">
+        <f>IF(ISBLANK(center_0!AA1),"",center_0!AA1)</f>
+        <v/>
+      </c>
+      <c r="AB1" t="str">
+        <f>IF(ISBLANK(center_0!AB1),"",center_0!AB1)</f>
+        <v/>
+      </c>
+      <c r="AC1" t="str">
+        <f>IF(ISBLANK(center_0!AC1),"",center_0!AC1)</f>
+        <v/>
+      </c>
+      <c r="AD1" t="str">
+        <f>IF(ISBLANK(center_0!AD1),"",center_0!AD1)</f>
+        <v/>
+      </c>
+      <c r="AE1" t="str">
+        <f>IF(ISBLANK(center_0!AE1),"",center_0!AE1)</f>
+        <v/>
+      </c>
+      <c r="AF1" t="str">
+        <f>IF(ISBLANK(center_0!AF1),"",center_0!AF1)</f>
+        <v/>
+      </c>
+      <c r="AG1" t="str">
+        <f>IF(ISBLANK(center_0!AG1),"",center_0!AG1)</f>
+        <v/>
+      </c>
+      <c r="AH1" t="str">
+        <f>IF(ISBLANK(center_0!AH1),"",center_0!AH1)</f>
+        <v/>
+      </c>
+      <c r="AI1" t="str">
+        <f>IF(ISBLANK(center_0!AI1),"",center_0!AI1)</f>
+        <v/>
+      </c>
+      <c r="AJ1" t="str">
+        <f>IF(ISBLANK(center_0!AJ1),"",center_0!AJ1)</f>
+        <v/>
+      </c>
+      <c r="AK1" t="str">
+        <f>IF(ISBLANK(center_0!AK1),"",center_0!AK1)</f>
+        <v/>
+      </c>
+      <c r="AL1" t="str">
+        <f>IF(ISBLANK(center_0!AL1),"",center_0!AL1)</f>
+        <v/>
+      </c>
+      <c r="AM1" t="str">
+        <f>IF(ISBLANK(center_0!AM1),"",center_0!AM1)</f>
+        <v/>
+      </c>
+      <c r="AN1" t="str">
+        <f>IF(ISBLANK(center_0!AN1),"",center_0!AN1)</f>
+        <v/>
+      </c>
+      <c r="AO1" t="str">
+        <f>IF(ISBLANK(center_0!AO1),"",center_0!AO1)</f>
+        <v/>
+      </c>
+      <c r="AP1" t="str">
+        <f>IF(ISBLANK(center_0!AP1),"",center_0!AP1)</f>
+        <v/>
+      </c>
+      <c r="AQ1" t="str">
+        <f>IF(ISBLANK(center_0!AQ1),"",center_0!AQ1)</f>
+        <v/>
+      </c>
+      <c r="AR1" t="str">
+        <f>IF(ISBLANK(center_0!AR1),"",center_0!AR1)</f>
+        <v/>
+      </c>
+      <c r="AS1" t="str">
+        <f>IF(ISBLANK(center_0!AS1),"",center_0!AS1)</f>
+        <v/>
+      </c>
+      <c r="AT1" t="str">
+        <f>IF(ISBLANK(center_0!AT1),"",center_0!AT1)</f>
+        <v/>
+      </c>
+      <c r="AU1" t="str">
+        <f>IF(ISBLANK(center_0!AU1),"",center_0!AU1)</f>
+        <v/>
+      </c>
+      <c r="AV1" t="str">
+        <f>IF(ISBLANK(center_0!AV1),"",center_0!AV1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
+        <v>gas</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
+        <v>CO2</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
+        <v>CO</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
+        <v>CO</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
+        <v>CO</v>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
+        <v>CO</v>
+      </c>
+      <c r="O2" t="str">
+        <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
+        <v>CO</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
+        <v>CO</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
+        <v>CO</v>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
+        <v>CO</v>
+      </c>
+      <c r="S2" t="str">
+        <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
+        <v>CO</v>
+      </c>
+      <c r="T2" t="str">
+        <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
+        <v>H2O</v>
+      </c>
+      <c r="U2" t="str">
+        <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
+        <v>H2O</v>
+      </c>
+      <c r="V2" t="str">
+        <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
+        <v>H2O</v>
+      </c>
+      <c r="W2" t="str">
+        <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
+        <v/>
+      </c>
+      <c r="X2" t="str">
+        <f>IF(ISBLANK(center_0!X2),"",center_0!X2)</f>
+        <v/>
+      </c>
+      <c r="Y2" t="str">
+        <f>IF(ISBLANK(center_0!Y2),"",center_0!Y2)</f>
+        <v/>
+      </c>
+      <c r="Z2" t="str">
+        <f>IF(ISBLANK(center_0!Z2),"",center_0!Z2)</f>
+        <v/>
+      </c>
+      <c r="AA2" t="str">
+        <f>IF(ISBLANK(center_0!AA2),"",center_0!AA2)</f>
+        <v/>
+      </c>
+      <c r="AB2" t="str">
+        <f>IF(ISBLANK(center_0!AB2),"",center_0!AB2)</f>
+        <v/>
+      </c>
+      <c r="AC2" t="str">
+        <f>IF(ISBLANK(center_0!AC2),"",center_0!AC2)</f>
+        <v/>
+      </c>
+      <c r="AD2" t="str">
+        <f>IF(ISBLANK(center_0!AD2),"",center_0!AD2)</f>
+        <v/>
+      </c>
+      <c r="AE2" t="str">
+        <f>IF(ISBLANK(center_0!AE2),"",center_0!AE2)</f>
+        <v/>
+      </c>
+      <c r="AF2" t="str">
+        <f>IF(ISBLANK(center_0!AF2),"",center_0!AF2)</f>
+        <v/>
+      </c>
+      <c r="AG2" t="str">
+        <f>IF(ISBLANK(center_0!AG2),"",center_0!AG2)</f>
+        <v/>
+      </c>
+      <c r="AH2" t="str">
+        <f>IF(ISBLANK(center_0!AH2),"",center_0!AH2)</f>
+        <v/>
+      </c>
+      <c r="AI2" t="str">
+        <f>IF(ISBLANK(center_0!AI2),"",center_0!AI2)</f>
+        <v/>
+      </c>
+      <c r="AJ2" t="str">
+        <f>IF(ISBLANK(center_0!AJ2),"",center_0!AJ2)</f>
+        <v/>
+      </c>
+      <c r="AK2" t="str">
+        <f>IF(ISBLANK(center_0!AK2),"",center_0!AK2)</f>
+        <v/>
+      </c>
+      <c r="AL2" t="str">
+        <f>IF(ISBLANK(center_0!AL2),"",center_0!AL2)</f>
+        <v/>
+      </c>
+      <c r="AM2" t="str">
+        <f>IF(ISBLANK(center_0!AM2),"",center_0!AM2)</f>
+        <v/>
+      </c>
+      <c r="AN2" t="str">
+        <f>IF(ISBLANK(center_0!AN2),"",center_0!AN2)</f>
+        <v/>
+      </c>
+      <c r="AO2" t="str">
+        <f>IF(ISBLANK(center_0!AO2),"",center_0!AO2)</f>
+        <v/>
+      </c>
+      <c r="AP2" t="str">
+        <f>IF(ISBLANK(center_0!AP2),"",center_0!AP2)</f>
+        <v/>
+      </c>
+      <c r="AQ2" t="str">
+        <f>IF(ISBLANK(center_0!AQ2),"",center_0!AQ2)</f>
+        <v/>
+      </c>
+      <c r="AR2" t="str">
+        <f>IF(ISBLANK(center_0!AR2),"",center_0!AR2)</f>
+        <v/>
+      </c>
+      <c r="AS2" t="str">
+        <f>IF(ISBLANK(center_0!AS2),"",center_0!AS2)</f>
+        <v/>
+      </c>
+      <c r="AT2" t="str">
+        <f>IF(ISBLANK(center_0!AT2),"",center_0!AT2)</f>
+        <v/>
+      </c>
+      <c r="AU2" t="str">
+        <f>IF(ISBLANK(center_0!AU2),"",center_0!AU2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
+        <v>almarri2009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
+        <v>ducuosso2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
+        <v>figueiredo1999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
+        <v>figueiredo2007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
+        <v>gorghulo2008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
+        <v>li2011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
+        <v>morales2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
+        <v>na2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
+        <v>samant2004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
+        <v>szymanski2002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
+        <v>zhou2007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
+        <v>almarri2009b</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
+        <v>saal2020a</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
+        <v>saal2020b</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B49426-40FA-4A8E-9024-66BDA98D0A8E}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -1677,7 +2933,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -1829,7 +3085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552C6DE0-A18F-46F1-A139-D60050F2DE41}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -2306,7 +3562,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -2458,7 +3714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0093193B-42D2-4CB5-99F9-AFD01B54638D}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -2939,7 +4195,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -3091,7 +4347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD939A53-4329-499E-A0E8-36AD8584F372}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -3572,7 +4828,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -4276,7 +5532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B2B75D-4D58-48A6-8AE4-061359CFFBFC}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -4757,7 +6013,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -4909,7 +6165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D46676C-6D47-439D-8E91-C7448FAFDD09}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -5390,7 +6646,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -5542,7 +6798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A734E0C-7A4B-428A-95DC-306859B6AB0F}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
@@ -6023,640 +7279,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <f>IF(ISBLANK(center_0!A18),"",center_0!A18)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <f>IF(ISBLANK(center_0!A19),"",center_0!A19)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <f>IF(ISBLANK(center_0!A20),"",center_0!A20)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f>IF(ISBLANK(center_0!A21),"",center_0!A21)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <f>IF(ISBLANK(center_0!A22),"",center_0!A22)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <f>IF(ISBLANK(center_0!A23),"",center_0!A23)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <f>IF(ISBLANK(center_0!A24),"",center_0!A24)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <f>IF(ISBLANK(center_0!A25),"",center_0!A25)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
-        <f>IF(ISBLANK(center_0!A26),"",center_0!A26)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <f>IF(ISBLANK(center_0!A27),"",center_0!A27)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <f>IF(ISBLANK(center_0!A28),"",center_0!A28)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <f>IF(ISBLANK(center_0!A29),"",center_0!A29)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <f>IF(ISBLANK(center_0!A30),"",center_0!A30)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <f>IF(ISBLANK(center_0!A31),"",center_0!A31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f>IF(ISBLANK(center_0!A32),"",center_0!A32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <f>IF(ISBLANK(center_0!A33),"",center_0!A33)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
-        <f>IF(ISBLANK(center_0!A34),"",center_0!A34)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <f>IF(ISBLANK(center_0!A35),"",center_0!A35)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="str">
-        <f>IF(ISBLANK(center_0!A36),"",center_0!A36)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="str">
-        <f>IF(ISBLANK(center_0!A37),"",center_0!A37)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="str">
-        <f>IF(ISBLANK(center_0!A38),"",center_0!A38)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="str">
-        <f>IF(ISBLANK(center_0!A39),"",center_0!A39)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="str">
-        <f>IF(ISBLANK(center_0!A40),"",center_0!A40)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="str">
-        <f>IF(ISBLANK(center_0!A41),"",center_0!A41)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C02276-5893-45C5-8032-5F138C27CB79}">
-  <dimension ref="A1:AV41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A1" t="str">
-        <f>IF(ISBLANK(center_0!A1),"",center_0!A1)</f>
-        <v>group</v>
-      </c>
-      <c r="B1" t="str">
-        <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
-      </c>
-      <c r="C1" t="str">
-        <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
-      </c>
-      <c r="D1" t="str">
-        <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
-      </c>
-      <c r="E1" t="str">
-        <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
-        <v>anhydrides</v>
-      </c>
-      <c r="F1" t="str">
-        <f>IF(ISBLANK(center_0!F1),"",center_0!F1)</f>
-        <v>peroxides</v>
-      </c>
-      <c r="G1" t="str">
-        <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
-      </c>
-      <c r="H1" t="str">
-        <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
-      </c>
-      <c r="I1" t="str">
-        <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
-      </c>
-      <c r="J1" t="str">
-        <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
-      </c>
-      <c r="K1" t="str">
-        <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
-      </c>
-      <c r="L1" t="str">
-        <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
-      </c>
-      <c r="M1" t="str">
-        <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
-        <v>anhydrides</v>
-      </c>
-      <c r="N1" t="str">
-        <f>IF(ISBLANK(center_0!N1),"",center_0!N1)</f>
-        <v>hydroxyl</v>
-      </c>
-      <c r="O1" t="str">
-        <f>IF(ISBLANK(center_0!O1),"",center_0!O1)</f>
-        <v>phenols</v>
-      </c>
-      <c r="P1" t="str">
-        <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
-      </c>
-      <c r="Q1" t="str">
-        <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
-      </c>
-      <c r="R1" t="str">
-        <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
-        <v>ether</v>
-      </c>
-      <c r="S1" t="str">
-        <f>IF(ISBLANK(center_0!S1),"",center_0!S1)</f>
-        <v>pyrones</v>
-      </c>
-      <c r="T1" t="str">
-        <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
-      </c>
-      <c r="U1" t="str">
-        <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
-      </c>
-      <c r="V1" t="str">
-        <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
-      </c>
-      <c r="W1" t="str">
-        <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
-        <v/>
-      </c>
-      <c r="X1" t="str">
-        <f>IF(ISBLANK(center_0!X1),"",center_0!X1)</f>
-        <v/>
-      </c>
-      <c r="Y1" t="str">
-        <f>IF(ISBLANK(center_0!Y1),"",center_0!Y1)</f>
-        <v/>
-      </c>
-      <c r="Z1" t="str">
-        <f>IF(ISBLANK(center_0!Z1),"",center_0!Z1)</f>
-        <v/>
-      </c>
-      <c r="AA1" t="str">
-        <f>IF(ISBLANK(center_0!AA1),"",center_0!AA1)</f>
-        <v/>
-      </c>
-      <c r="AB1" t="str">
-        <f>IF(ISBLANK(center_0!AB1),"",center_0!AB1)</f>
-        <v/>
-      </c>
-      <c r="AC1" t="str">
-        <f>IF(ISBLANK(center_0!AC1),"",center_0!AC1)</f>
-        <v/>
-      </c>
-      <c r="AD1" t="str">
-        <f>IF(ISBLANK(center_0!AD1),"",center_0!AD1)</f>
-        <v/>
-      </c>
-      <c r="AE1" t="str">
-        <f>IF(ISBLANK(center_0!AE1),"",center_0!AE1)</f>
-        <v/>
-      </c>
-      <c r="AF1" t="str">
-        <f>IF(ISBLANK(center_0!AF1),"",center_0!AF1)</f>
-        <v/>
-      </c>
-      <c r="AG1" t="str">
-        <f>IF(ISBLANK(center_0!AG1),"",center_0!AG1)</f>
-        <v/>
-      </c>
-      <c r="AH1" t="str">
-        <f>IF(ISBLANK(center_0!AH1),"",center_0!AH1)</f>
-        <v/>
-      </c>
-      <c r="AI1" t="str">
-        <f>IF(ISBLANK(center_0!AI1),"",center_0!AI1)</f>
-        <v/>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IF(ISBLANK(center_0!AJ1),"",center_0!AJ1)</f>
-        <v/>
-      </c>
-      <c r="AK1" t="str">
-        <f>IF(ISBLANK(center_0!AK1),"",center_0!AK1)</f>
-        <v/>
-      </c>
-      <c r="AL1" t="str">
-        <f>IF(ISBLANK(center_0!AL1),"",center_0!AL1)</f>
-        <v/>
-      </c>
-      <c r="AM1" t="str">
-        <f>IF(ISBLANK(center_0!AM1),"",center_0!AM1)</f>
-        <v/>
-      </c>
-      <c r="AN1" t="str">
-        <f>IF(ISBLANK(center_0!AN1),"",center_0!AN1)</f>
-        <v/>
-      </c>
-      <c r="AO1" t="str">
-        <f>IF(ISBLANK(center_0!AO1),"",center_0!AO1)</f>
-        <v/>
-      </c>
-      <c r="AP1" t="str">
-        <f>IF(ISBLANK(center_0!AP1),"",center_0!AP1)</f>
-        <v/>
-      </c>
-      <c r="AQ1" t="str">
-        <f>IF(ISBLANK(center_0!AQ1),"",center_0!AQ1)</f>
-        <v/>
-      </c>
-      <c r="AR1" t="str">
-        <f>IF(ISBLANK(center_0!AR1),"",center_0!AR1)</f>
-        <v/>
-      </c>
-      <c r="AS1" t="str">
-        <f>IF(ISBLANK(center_0!AS1),"",center_0!AS1)</f>
-        <v/>
-      </c>
-      <c r="AT1" t="str">
-        <f>IF(ISBLANK(center_0!AT1),"",center_0!AT1)</f>
-        <v/>
-      </c>
-      <c r="AU1" t="str">
-        <f>IF(ISBLANK(center_0!AU1),"",center_0!AU1)</f>
-        <v/>
-      </c>
-      <c r="AV1" t="str">
-        <f>IF(ISBLANK(center_0!AV1),"",center_0!AV1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>IF(ISBLANK(center_0!A2),"",center_0!A2)</f>
-        <v>gas</v>
-      </c>
-      <c r="B2" t="str">
-        <f>IF(ISBLANK(center_0!B2),"",center_0!B2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="C2" t="str">
-        <f>IF(ISBLANK(center_0!C2),"",center_0!C2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(ISBLANK(center_0!D2),"",center_0!D2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="E2" t="str">
-        <f>IF(ISBLANK(center_0!E2),"",center_0!E2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="F2" t="str">
-        <f>IF(ISBLANK(center_0!F2),"",center_0!F2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(ISBLANK(center_0!G2),"",center_0!G2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="H2" t="str">
-        <f>IF(ISBLANK(center_0!H2),"",center_0!H2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="I2" t="str">
-        <f>IF(ISBLANK(center_0!I2),"",center_0!I2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="J2" t="str">
-        <f>IF(ISBLANK(center_0!J2),"",center_0!J2)</f>
-        <v>CO2</v>
-      </c>
-      <c r="K2" t="str">
-        <f>IF(ISBLANK(center_0!K2),"",center_0!K2)</f>
-        <v>CO</v>
-      </c>
-      <c r="L2" t="str">
-        <f>IF(ISBLANK(center_0!L2),"",center_0!L2)</f>
-        <v>CO</v>
-      </c>
-      <c r="M2" t="str">
-        <f>IF(ISBLANK(center_0!M2),"",center_0!M2)</f>
-        <v>CO</v>
-      </c>
-      <c r="N2" t="str">
-        <f>IF(ISBLANK(center_0!N2),"",center_0!N2)</f>
-        <v>CO</v>
-      </c>
-      <c r="O2" t="str">
-        <f>IF(ISBLANK(center_0!O2),"",center_0!O2)</f>
-        <v>CO</v>
-      </c>
-      <c r="P2" t="str">
-        <f>IF(ISBLANK(center_0!P2),"",center_0!P2)</f>
-        <v>CO</v>
-      </c>
-      <c r="Q2" t="str">
-        <f>IF(ISBLANK(center_0!Q2),"",center_0!Q2)</f>
-        <v>CO</v>
-      </c>
-      <c r="R2" t="str">
-        <f>IF(ISBLANK(center_0!R2),"",center_0!R2)</f>
-        <v>CO</v>
-      </c>
-      <c r="S2" t="str">
-        <f>IF(ISBLANK(center_0!S2),"",center_0!S2)</f>
-        <v>CO</v>
-      </c>
-      <c r="T2" t="str">
-        <f>IF(ISBLANK(center_0!T2),"",center_0!T2)</f>
-        <v>H2O</v>
-      </c>
-      <c r="U2" t="str">
-        <f>IF(ISBLANK(center_0!U2),"",center_0!U2)</f>
-        <v>H2O</v>
-      </c>
-      <c r="V2" t="str">
-        <f>IF(ISBLANK(center_0!V2),"",center_0!V2)</f>
-        <v>H2O</v>
-      </c>
-      <c r="W2" t="str">
-        <f>IF(ISBLANK(center_0!W2),"",center_0!W2)</f>
-        <v/>
-      </c>
-      <c r="X2" t="str">
-        <f>IF(ISBLANK(center_0!X2),"",center_0!X2)</f>
-        <v/>
-      </c>
-      <c r="Y2" t="str">
-        <f>IF(ISBLANK(center_0!Y2),"",center_0!Y2)</f>
-        <v/>
-      </c>
-      <c r="Z2" t="str">
-        <f>IF(ISBLANK(center_0!Z2),"",center_0!Z2)</f>
-        <v/>
-      </c>
-      <c r="AA2" t="str">
-        <f>IF(ISBLANK(center_0!AA2),"",center_0!AA2)</f>
-        <v/>
-      </c>
-      <c r="AB2" t="str">
-        <f>IF(ISBLANK(center_0!AB2),"",center_0!AB2)</f>
-        <v/>
-      </c>
-      <c r="AC2" t="str">
-        <f>IF(ISBLANK(center_0!AC2),"",center_0!AC2)</f>
-        <v/>
-      </c>
-      <c r="AD2" t="str">
-        <f>IF(ISBLANK(center_0!AD2),"",center_0!AD2)</f>
-        <v/>
-      </c>
-      <c r="AE2" t="str">
-        <f>IF(ISBLANK(center_0!AE2),"",center_0!AE2)</f>
-        <v/>
-      </c>
-      <c r="AF2" t="str">
-        <f>IF(ISBLANK(center_0!AF2),"",center_0!AF2)</f>
-        <v/>
-      </c>
-      <c r="AG2" t="str">
-        <f>IF(ISBLANK(center_0!AG2),"",center_0!AG2)</f>
-        <v/>
-      </c>
-      <c r="AH2" t="str">
-        <f>IF(ISBLANK(center_0!AH2),"",center_0!AH2)</f>
-        <v/>
-      </c>
-      <c r="AI2" t="str">
-        <f>IF(ISBLANK(center_0!AI2),"",center_0!AI2)</f>
-        <v/>
-      </c>
-      <c r="AJ2" t="str">
-        <f>IF(ISBLANK(center_0!AJ2),"",center_0!AJ2)</f>
-        <v/>
-      </c>
-      <c r="AK2" t="str">
-        <f>IF(ISBLANK(center_0!AK2),"",center_0!AK2)</f>
-        <v/>
-      </c>
-      <c r="AL2" t="str">
-        <f>IF(ISBLANK(center_0!AL2),"",center_0!AL2)</f>
-        <v/>
-      </c>
-      <c r="AM2" t="str">
-        <f>IF(ISBLANK(center_0!AM2),"",center_0!AM2)</f>
-        <v/>
-      </c>
-      <c r="AN2" t="str">
-        <f>IF(ISBLANK(center_0!AN2),"",center_0!AN2)</f>
-        <v/>
-      </c>
-      <c r="AO2" t="str">
-        <f>IF(ISBLANK(center_0!AO2),"",center_0!AO2)</f>
-        <v/>
-      </c>
-      <c r="AP2" t="str">
-        <f>IF(ISBLANK(center_0!AP2),"",center_0!AP2)</f>
-        <v/>
-      </c>
-      <c r="AQ2" t="str">
-        <f>IF(ISBLANK(center_0!AQ2),"",center_0!AQ2)</f>
-        <v/>
-      </c>
-      <c r="AR2" t="str">
-        <f>IF(ISBLANK(center_0!AR2),"",center_0!AR2)</f>
-        <v/>
-      </c>
-      <c r="AS2" t="str">
-        <f>IF(ISBLANK(center_0!AS2),"",center_0!AS2)</f>
-        <v/>
-      </c>
-      <c r="AT2" t="str">
-        <f>IF(ISBLANK(center_0!AT2),"",center_0!AT2)</f>
-        <v/>
-      </c>
-      <c r="AU2" t="str">
-        <f>IF(ISBLANK(center_0!AU2),"",center_0!AU2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>IF(ISBLANK(center_0!A3),"",center_0!A3)</f>
-        <v>almarri2009</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>IF(ISBLANK(center_0!A4),"",center_0!A4)</f>
-        <v>ducuosso2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>IF(ISBLANK(center_0!A5),"",center_0!A5)</f>
-        <v>figueiredo1999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>IF(ISBLANK(center_0!A6),"",center_0!A6)</f>
-        <v>figueiredo2007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>IF(ISBLANK(center_0!A7),"",center_0!A7)</f>
-        <v>gorghulo2008</v>
-      </c>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
-      </c>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
-      </c>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>IF(ISBLANK(center_0!A11),"",center_0!A11)</f>
-        <v>samant2004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f>IF(ISBLANK(center_0!A12),"",center_0!A12)</f>
-        <v>szymanski2002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f>IF(ISBLANK(center_0!A13),"",center_0!A13)</f>
-        <v>zhou2007</v>
-      </c>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f>IF(ISBLANK(center_0!A14),"",center_0!A14)</f>
-        <v>almarri2009b</v>
-      </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>saal2020a</v>
-      </c>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v>saal2020b</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v>test</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Bugfixes in robustness and reworking of IR-corrections
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Documents\GitHub\TGA-FTIR-hyphenation-tool-kit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CCDB66-6FB6-4972-B182-F716BFA6F762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66049CA2-F57B-4F63-877B-1BCDE24FAF7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
   <sheets>
     <sheet name="center_0" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>figueiredo1999</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>H2O</t>
+  </si>
+  <si>
+    <t>wh</t>
   </si>
 </sst>
 </file>
@@ -546,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E64D511-D4ED-4E7F-BCBD-B5A2B90CC7A9}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1823,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55AB40E-2FFC-42C2-AD78-D9FFEE5C8809}">
   <dimension ref="A1:AV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2290,11 +2293,17 @@
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
         <v>saal2020a</v>
       </c>
+      <c r="M15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
         <v>saal2020b</v>
+      </c>
+      <c r="M16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Slight name modification of groups
for more individueal evaluations
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddittman\Downloads\8PAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0C4E9D-0696-42A3-9391-8EE7A6AE0658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341BC6B5-625B-431F-8546-2EBB9770305C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="685" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>figueiredo1999</t>
   </si>
@@ -122,18 +122,6 @@
     <t>group</t>
   </si>
   <si>
-    <t>adsorbed</t>
-  </si>
-  <si>
-    <t>unassigned</t>
-  </si>
-  <si>
-    <t>unassigned 1</t>
-  </si>
-  <si>
-    <t>unassigned 2</t>
-  </si>
-  <si>
     <t>almarri2009b</t>
   </si>
   <si>
@@ -153,6 +141,21 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>adsorbed-CO2</t>
+  </si>
+  <si>
+    <t>unassigned-CO2</t>
+  </si>
+  <si>
+    <t>adsorbed-H2O</t>
+  </si>
+  <si>
+    <t>unassigned-H2O 1</t>
+  </si>
+  <si>
+    <t>unassigned-H2O 2</t>
   </si>
 </sst>
 </file>
@@ -556,16 +559,16 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -587,7 +590,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -602,7 +605,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>15</v>
@@ -641,13 +644,13 @@
         <v>5</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -655,67 +658,67 @@
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1054,7 +1057,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>95</v>
@@ -1101,7 +1104,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>95</v>
@@ -1198,7 +1201,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -1218,7 +1221,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -1270,15 +1273,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -1898,29 +1901,28 @@
   <dimension ref="A1:AV39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11.44140625" style="1"/>
-    <col min="13" max="13" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
@@ -1931,7 +1933,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -1951,7 +1953,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -2003,15 +2005,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -2332,7 +2334,7 @@
         <v>figueiredo2007</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.3">
@@ -2400,7 +2402,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -2593,7 +2595,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -2613,7 +2615,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -2665,15 +2667,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -3326,7 +3328,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -3346,7 +3348,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -3398,15 +3400,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -4055,7 +4057,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -4075,7 +4077,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -4127,15 +4129,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -4956,7 +4958,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -4976,7 +4978,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -5028,15 +5030,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -6241,7 +6243,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -6261,7 +6263,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -6313,15 +6315,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -6974,7 +6976,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -6994,7 +6996,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -7046,15 +7048,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -7875,7 +7877,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
@@ -7895,7 +7897,7 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned</v>
+        <v>unassigned-CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
@@ -7947,15 +7949,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed</v>
+        <v>adsorbed-H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned 1</v>
+        <v>unassigned-H2O 1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned 2</v>
+        <v>unassigned-H2O 2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>

</xml_diff>

<commit_message>
method distinguished in a, b, c
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddittman\Downloads\8PAC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddittman\Downloads\8PAC_washed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341BC6B5-625B-431F-8546-2EBB9770305C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26F1964-A890-4CF9-AE1E-EE42DA23641A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="685" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>figueiredo1999</t>
   </si>
@@ -137,9 +137,6 @@
     <t>wh</t>
   </si>
   <si>
-    <t>dittmann2021</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -156,6 +153,15 @@
   </si>
   <si>
     <t>unassigned-H2O 2</t>
+  </si>
+  <si>
+    <t>dittmann2021a</t>
+  </si>
+  <si>
+    <t>dittmann2021b</t>
+  </si>
+  <si>
+    <t>dittmann2021c</t>
   </si>
 </sst>
 </file>
@@ -234,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -242,6 +248,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -556,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E64D511-D4ED-4E7F-BCBD-B5A2B90CC7A9}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,7 +597,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -605,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>15</v>
@@ -644,13 +651,13 @@
         <v>5</v>
       </c>
       <c r="T1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1104,7 +1111,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1">
         <v>95</v>
@@ -1153,6 +1160,103 @@
       </c>
       <c r="V15" s="1">
         <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1">
+        <v>245</v>
+      </c>
+      <c r="D16" s="1">
+        <v>380</v>
+      </c>
+      <c r="E16" s="1">
+        <v>500</v>
+      </c>
+      <c r="H16" s="3">
+        <v>635</v>
+      </c>
+      <c r="I16" s="3">
+        <v>785</v>
+      </c>
+      <c r="K16" s="3">
+        <v>255</v>
+      </c>
+      <c r="L16" s="3">
+        <v>410</v>
+      </c>
+      <c r="M16" s="1">
+        <v>530</v>
+      </c>
+      <c r="O16" s="3">
+        <v>670</v>
+      </c>
+      <c r="P16" s="3">
+        <v>790</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>870</v>
+      </c>
+      <c r="S16" s="1">
+        <v>960</v>
+      </c>
+      <c r="T16" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1">
+        <v>245</v>
+      </c>
+      <c r="D17" s="1">
+        <v>380</v>
+      </c>
+      <c r="E17" s="1">
+        <v>500</v>
+      </c>
+      <c r="G17" s="7">
+        <v>600</v>
+      </c>
+      <c r="H17" s="3">
+        <v>635</v>
+      </c>
+      <c r="I17" s="3">
+        <v>785</v>
+      </c>
+      <c r="K17" s="3">
+        <v>255</v>
+      </c>
+      <c r="L17" s="3">
+        <v>410</v>
+      </c>
+      <c r="M17" s="1">
+        <v>530</v>
+      </c>
+      <c r="O17" s="3">
+        <v>670</v>
+      </c>
+      <c r="P17" s="3">
+        <v>790</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>870</v>
+      </c>
+      <c r="S17" s="1">
+        <v>960</v>
+      </c>
+      <c r="T17" s="1">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1764,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),1,"")</f>
@@ -1750,13 +1854,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -2334,7 +2438,7 @@
         <v>figueiredo2007</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.3">
@@ -2395,7 +2499,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2411,13 +2515,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -3054,7 +3158,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),47.5,"")</f>
@@ -3144,13 +3248,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -3783,7 +3887,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),0.5,"")</f>
@@ -3873,13 +3977,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -4684,7 +4788,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),center_0!B15-30,"")</f>
@@ -4774,13 +4878,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -5417,7 +5521,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),0,"")</f>
@@ -5507,13 +5611,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -6702,7 +6806,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),0,"")</f>
@@ -6792,13 +6896,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -7603,7 +7707,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),center_0!B15+30,"")</f>
@@ -7693,13 +7797,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -8336,7 +8440,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>IF(ISBLANK(center_0!A15),"",center_0!A15)</f>
-        <v>dittmann2021</v>
+        <v>dittmann2021a</v>
       </c>
       <c r="B15" s="1">
         <f>IF(ISNUMBER(center_0!B15),95,"")</f>
@@ -8426,13 +8530,13 @@
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>IF(ISBLANK(center_0!A16),"",center_0!A16)</f>
-        <v/>
+        <v>dittmann2021b</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>dittmann2021c</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changes in group names
underscore now delimits groups of the same name but with addional fittings.
"carboxylic" is renamed to "carboxylic acids"
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddittman\Desktop\Paper - Aktivkohlecharakterisierung\06_TGA-FTIR\TGA-FTIR-hyphenation-tool-kit-master_8PAC_washed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE1A934-A978-4D07-B6B4-0978BE1224A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B098804-8D70-4F4D-B274-B15540F2FFC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="685" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
@@ -83,24 +83,6 @@
     <t>szymanski2002</t>
   </si>
   <si>
-    <t>carboxylic 1</t>
-  </si>
-  <si>
-    <t>carboxylic 2</t>
-  </si>
-  <si>
-    <t>lactones 1</t>
-  </si>
-  <si>
-    <t>lactones 2</t>
-  </si>
-  <si>
-    <t>carbonyls 1</t>
-  </si>
-  <si>
-    <t>carbonyls 2</t>
-  </si>
-  <si>
     <t>gas</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
   </si>
   <si>
     <t>almarri2009</t>
-  </si>
-  <si>
-    <t>carbonyl 1</t>
   </si>
   <si>
     <t>ducuosso2015</t>
@@ -137,21 +116,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>adsorbed-CO2</t>
-  </si>
-  <si>
-    <t>unassigned-CO2</t>
-  </si>
-  <si>
-    <t>adsorbed-H2O</t>
-  </si>
-  <si>
-    <t>unassigned-H2O 1</t>
-  </si>
-  <si>
-    <t>unassigned-H2O 2</t>
-  </si>
-  <si>
     <t>dittmann2021a</t>
   </si>
   <si>
@@ -159,6 +123,42 @@
   </si>
   <si>
     <t>dittmann2021c</t>
+  </si>
+  <si>
+    <t>adsorbed CO2</t>
+  </si>
+  <si>
+    <t>carboxylic acids_1</t>
+  </si>
+  <si>
+    <t>carboxylic acids_2</t>
+  </si>
+  <si>
+    <t>unassigned CO2</t>
+  </si>
+  <si>
+    <t>lactones_1</t>
+  </si>
+  <si>
+    <t>lactones_2</t>
+  </si>
+  <si>
+    <t>carbonyls_1</t>
+  </si>
+  <si>
+    <t>carbonyls_2</t>
+  </si>
+  <si>
+    <t>unassigned H2O_1</t>
+  </si>
+  <si>
+    <t>adsorbed H2O</t>
+  </si>
+  <si>
+    <t>unassigned H2O_2</t>
+  </si>
+  <si>
+    <t>carbonyls</t>
   </si>
 </sst>
 </file>
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -268,6 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -585,44 +586,43 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -631,37 +631,37 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>10</v>
@@ -670,86 +670,86 @@
         <v>5</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>250</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>390</v>
@@ -934,34 +934,43 @@
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="10">
         <v>263.66666666666663</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="10">
         <v>377.16666666666663</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="10">
         <v>665.66666666666663</v>
       </c>
-      <c r="H9" s="1">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
         <v>665.66666666666663</v>
       </c>
-      <c r="M9" s="1">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10">
         <v>665.66666666666663</v>
       </c>
-      <c r="O9" s="1">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <v>699.5</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="10">
         <v>867.83333333333326</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="10">
         <v>1090</v>
       </c>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>280</v>
@@ -1083,7 +1092,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
         <v>95</v>
@@ -1136,7 +1145,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
         <v>95</v>
@@ -1183,7 +1192,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1">
         <v>95</v>
@@ -1244,28 +1253,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -1276,15 +1285,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -1296,27 +1305,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -1332,11 +1341,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -1348,15 +1357,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -2131,28 +2140,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -2163,15 +2172,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -2183,27 +2192,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -2219,11 +2228,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -2235,15 +2244,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -2564,7 +2573,7 @@
         <v>figueiredo2007</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
@@ -2619,7 +2628,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2631,7 +2640,7 @@
         <v>dittmann2021b</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
@@ -2640,7 +2649,7 @@
         <v>dittmann2021c</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -2785,28 +2794,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -2817,15 +2826,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -2837,27 +2846,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -2873,11 +2882,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -2889,15 +2898,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -3671,28 +3680,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -3703,15 +3712,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -3723,27 +3732,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -3759,11 +3768,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -3775,15 +3784,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -4554,28 +4563,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -4586,15 +4595,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -4606,27 +4615,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -4642,11 +4651,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -4658,15 +4667,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -5609,28 +5618,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -5641,15 +5650,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -5661,27 +5670,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -5697,11 +5706,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -5713,15 +5722,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -7047,28 +7056,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -7079,15 +7088,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -7099,27 +7108,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -7135,11 +7144,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -7151,15 +7160,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -7934,28 +7943,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -7966,15 +7975,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -7986,27 +7995,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -8022,11 +8031,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -8038,15 +8047,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>
@@ -8989,28 +8998,28 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -9021,15 +9030,15 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>IF(ISBLANK(center_0!B1),"",center_0!B1)</f>
-        <v>adsorbed-CO2</v>
+        <v>adsorbed CO2</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>IF(ISBLANK(center_0!C1),"",center_0!C1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="D1" s="4" t="str">
         <f>IF(ISBLANK(center_0!D1),"",center_0!D1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>IF(ISBLANK(center_0!E1),"",center_0!E1)</f>
@@ -9041,27 +9050,27 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>IF(ISBLANK(center_0!G1),"",center_0!G1)</f>
-        <v>unassigned-CO2</v>
+        <v>unassigned CO2</v>
       </c>
       <c r="H1" s="4" t="str">
         <f>IF(ISBLANK(center_0!H1),"",center_0!H1)</f>
-        <v>lactones 1</v>
+        <v>lactones_1</v>
       </c>
       <c r="I1" s="4" t="str">
         <f>IF(ISBLANK(center_0!I1),"",center_0!I1)</f>
-        <v>lactones 2</v>
+        <v>lactones_2</v>
       </c>
       <c r="J1" s="4" t="str">
         <f>IF(ISBLANK(center_0!J1),"",center_0!J1)</f>
-        <v>carbonyl 1</v>
+        <v>carbonyls</v>
       </c>
       <c r="K1" s="4" t="str">
         <f>IF(ISBLANK(center_0!K1),"",center_0!K1)</f>
-        <v>carboxylic 1</v>
+        <v>carboxylic acids_1</v>
       </c>
       <c r="L1" s="4" t="str">
         <f>IF(ISBLANK(center_0!L1),"",center_0!L1)</f>
-        <v>carboxylic 2</v>
+        <v>carboxylic acids_2</v>
       </c>
       <c r="M1" s="4" t="str">
         <f>IF(ISBLANK(center_0!M1),"",center_0!M1)</f>
@@ -9077,11 +9086,11 @@
       </c>
       <c r="P1" s="4" t="str">
         <f>IF(ISBLANK(center_0!P1),"",center_0!P1)</f>
-        <v>carbonyls 1</v>
+        <v>carbonyls_1</v>
       </c>
       <c r="Q1" s="4" t="str">
         <f>IF(ISBLANK(center_0!Q1),"",center_0!Q1)</f>
-        <v>carbonyls 2</v>
+        <v>carbonyls_2</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>IF(ISBLANK(center_0!R1),"",center_0!R1)</f>
@@ -9093,15 +9102,15 @@
       </c>
       <c r="T1" s="4" t="str">
         <f>IF(ISBLANK(center_0!T1),"",center_0!T1)</f>
-        <v>adsorbed-H2O</v>
+        <v>adsorbed H2O</v>
       </c>
       <c r="U1" s="4" t="str">
         <f>IF(ISBLANK(center_0!U1),"",center_0!U1)</f>
-        <v>unassigned-H2O 1</v>
+        <v>unassigned H2O_1</v>
       </c>
       <c r="V1" s="4" t="str">
         <f>IF(ISBLANK(center_0!V1),"",center_0!V1)</f>
-        <v>unassigned-H2O 2</v>
+        <v>unassigned H2O_2</v>
       </c>
       <c r="W1" s="4" t="str">
         <f>IF(ISBLANK(center_0!W1),"",center_0!W1)</f>

</xml_diff>

<commit_message>
li2011a and li2011b added
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddittman\Desktop\Paper - Aktivkohlecharakterisierung\06_TGA-FTIR\TGA-FTIR-hyphenation-tool-kit-master_8PAC_washed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73083D99-2309-4CA3-96FC-A6CD41B1B5A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B039EACE-F01F-4AD8-9AB9-9D745961F528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="685" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>figueiredo2007</t>
   </si>
   <si>
-    <t>li2011</t>
-  </si>
-  <si>
     <t>pyrones</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
   </si>
   <si>
     <t>gas</t>
-  </si>
-  <si>
-    <t>na2011</t>
   </si>
   <si>
     <t>almarri2009</t>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>ducousso2015</t>
+  </si>
+  <si>
+    <t>li2011b</t>
+  </si>
+  <si>
+    <t>li2011a</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E64D511-D4ED-4E7F-BCBD-B5A2B90CC7A9}">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -613,143 +613,143 @@
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>250</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1">
         <v>390</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1">
         <v>257</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1">
         <v>245</v>
@@ -932,83 +932,83 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10">
-        <v>263.66666666666663</v>
-      </c>
-      <c r="D9" s="10">
-        <v>377.16666666666663</v>
-      </c>
-      <c r="E9" s="10">
-        <v>665.66666666666663</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10">
-        <v>665.66666666666663</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10">
-        <v>665.66666666666663</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10">
-        <v>699.5</v>
-      </c>
-      <c r="P9" s="10">
-        <v>867.83333333333326</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>1090</v>
-      </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>280</v>
+      </c>
+      <c r="D9" s="1">
+        <v>400</v>
+      </c>
+      <c r="E9" s="1">
+        <v>540</v>
+      </c>
+      <c r="H9" s="1">
+        <v>650</v>
+      </c>
+      <c r="I9" s="1">
+        <v>800</v>
+      </c>
+      <c r="K9" s="1">
+        <v>300</v>
+      </c>
+      <c r="L9" s="1">
+        <v>420</v>
+      </c>
+      <c r="M9" s="1">
+        <v>550</v>
+      </c>
+      <c r="O9" s="1">
+        <v>680</v>
+      </c>
+      <c r="P9" s="1">
+        <v>800</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1020</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1">
-        <v>280</v>
-      </c>
-      <c r="D10" s="1">
-        <v>400</v>
-      </c>
-      <c r="E10" s="1">
-        <v>540</v>
-      </c>
-      <c r="H10" s="1">
-        <v>650</v>
-      </c>
-      <c r="I10" s="1">
-        <v>800</v>
-      </c>
-      <c r="K10" s="1">
-        <v>300</v>
-      </c>
-      <c r="L10" s="1">
-        <v>420</v>
-      </c>
-      <c r="M10" s="1">
-        <v>550</v>
-      </c>
-      <c r="O10" s="1">
-        <v>680</v>
-      </c>
-      <c r="P10" s="1">
-        <v>800</v>
-      </c>
-      <c r="S10" s="1">
-        <v>1020</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C10" s="10">
+        <v>263.66666666666663</v>
+      </c>
+      <c r="D10" s="10">
+        <v>377.16666666666663</v>
+      </c>
+      <c r="E10" s="10">
+        <v>665.66666666666663</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
+        <v>665.66666666666663</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10">
+        <v>665.66666666666663</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10">
+        <v>699.5</v>
+      </c>
+      <c r="P10" s="10">
+        <v>867.83333333333326</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>1090</v>
+      </c>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
         <v>291</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1">
         <v>427</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="13" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="9">
         <v>275</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>95</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>95</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>95</v>
@@ -1239,6 +1239,25 @@
       <c r="T16" s="1">
         <v>90</v>
       </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V13">
@@ -1695,19 +1714,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -2573,7 +2592,7 @@
         <v>figueiredo2007</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
@@ -2585,19 +2604,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -2628,7 +2647,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2640,7 +2659,7 @@
         <v>dittmann2021b</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
@@ -2649,7 +2668,7 @@
         <v>dittmann2021c</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -3236,19 +3255,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -4118,19 +4137,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -5089,19 +5108,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -6060,19 +6079,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -7498,19 +7517,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -8469,19 +8488,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -9440,19 +9459,19 @@
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>IF(ISBLANK(center_0!A8),"",center_0!A8)</f>
-        <v>li2011</v>
+        <v>li2011a</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>IF(ISBLANK(center_0!A9),"",center_0!A9)</f>
-        <v>morales2014</v>
+        <v>li2011b</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>IF(ISBLANK(center_0!A10),"",center_0!A10)</f>
-        <v>na2011</v>
+        <v>morales2014</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Restructuring of code, GUI
</commit_message>
<xml_diff>
--- a/Fitting_parameter.xlsx
+++ b/Fitting_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddittman\Desktop\Paper - Aktivkohlecharakterisierung\06_TGA-FTIR\TGA-FTIR-hyphenation-tool-kit-master_8PAC_washed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UBA_Promotion\3_TGA_FTIR\TGA-FTIR-hyphenation-tool-kit\TGA_FTIR_tools\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B039EACE-F01F-4AD8-9AB9-9D745961F528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD7246F-FE6A-4196-B262-B706AA4F13FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="685" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="685" xr2:uid="{BEEF2067-4EA6-4258-BE20-4BC7D06DB951}"/>
   </bookViews>
   <sheets>
     <sheet name="center_0" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>figueiredo1999</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>li2011a</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1243,30 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1">
+        <v>245</v>
+      </c>
+      <c r="D17" s="1">
+        <v>380</v>
+      </c>
+      <c r="E17" s="1">
+        <v>500</v>
+      </c>
+      <c r="K17" s="3">
+        <v>255</v>
+      </c>
+      <c r="L17" s="3">
+        <v>410</v>
+      </c>
+      <c r="M17" s="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -2020,7 +2046,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -2674,7 +2700,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -3560,7 +3586,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -4443,7 +4469,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -5498,7 +5524,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -6384,7 +6410,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -7823,7 +7849,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -8878,7 +8904,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -9764,7 +9790,7 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>IF(ISBLANK(center_0!A17),"",center_0!A17)</f>
-        <v/>
+        <v>test</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>